<commit_message>
correções simples, planilhas datas
</commit_message>
<xml_diff>
--- a/rh/FORMULÁRIO DISTRATO RCA.xlsx
+++ b/rh/FORMULÁRIO DISTRATO RCA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMERCIAL 04\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Analista Comercial\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C8B1CA-DA5B-4DF9-BECB-F89E428A0305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67296323-103D-4ABB-92AD-0F916F035F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rescisão-RCA" sheetId="13" r:id="rId1"/>
@@ -628,10 +628,10 @@
     <t xml:space="preserve">TITULAR </t>
   </si>
   <si>
+    <t>Analista de Dp</t>
+  </si>
+  <si>
     <t>CARLOS ALBERTO DA COSTA</t>
-  </si>
-  <si>
-    <t>Gerente de RH</t>
   </si>
 </sst>
 </file>
@@ -2772,8 +2772,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3449,7 +3449,7 @@
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="53"/>
       <c r="B38" s="134" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C38" s="134"/>
       <c r="D38" s="55"/>
@@ -3459,7 +3459,7 @@
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="53"/>
       <c r="B39" s="134" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="134"/>
       <c r="D39" s="55"/>
@@ -3499,8 +3499,8 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="B1:AC28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3746,9 +3746,9 @@
       <c r="E12" s="9"/>
     </row>
     <row r="14" spans="2:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="160">
-        <f>'Rescisão-RCA'!B31</f>
-        <v>0</v>
+      <c r="B14" s="160" t="str">
+        <f>"Fortaleza, " &amp; TEXT('Rescisão-RCA'!C10, "dd ""de"" mmmm ""de"" aaaa")</f>
+        <v>Fortaleza, 00 de janeiro de 1900</v>
       </c>
       <c r="C14" s="160"/>
       <c r="D14" s="160"/>

</xml_diff>

<commit_message>
correções simples, planilhas datas 1
</commit_message>
<xml_diff>
--- a/rh/FORMULÁRIO DISTRATO RCA.xlsx
+++ b/rh/FORMULÁRIO DISTRATO RCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Analista Comercial\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67296323-103D-4ABB-92AD-0F916F035F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EF15C1-0D1F-4BD5-83B6-D2689956151B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1781,6 +1781,36 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1797,36 +1827,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2772,8 +2772,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3373,9 +3373,9 @@
     </row>
     <row r="31" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="53"/>
-      <c r="B31" s="133">
-        <f>C10</f>
-        <v>0</v>
+      <c r="B31" s="133" t="str">
+        <f>TEXT(C10, "dd ""de"" mmmm ""de"" aaaa")</f>
+        <v>00 de janeiro de 1900</v>
       </c>
       <c r="C31" s="126"/>
       <c r="D31" s="79"/>
@@ -3500,7 +3500,7 @@
   <dimension ref="B1:AC28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="B14" sqref="B14:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3517,43 +3517,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="Q1" s="155" t="s">
+      <c r="Q1" s="152" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="156"/>
-      <c r="S1" s="156"/>
-      <c r="T1" s="156"/>
-      <c r="U1" s="157"/>
-      <c r="V1" s="145" t="s">
+      <c r="R1" s="153"/>
+      <c r="S1" s="153"/>
+      <c r="T1" s="153"/>
+      <c r="U1" s="154"/>
+      <c r="V1" s="155" t="s">
         <v>65</v>
       </c>
-      <c r="W1" s="146"/>
-      <c r="X1" s="146"/>
-      <c r="Y1" s="146"/>
-      <c r="Z1" s="147"/>
-      <c r="AA1" s="148" t="s">
+      <c r="W1" s="156"/>
+      <c r="X1" s="156"/>
+      <c r="Y1" s="156"/>
+      <c r="Z1" s="157"/>
+      <c r="AA1" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="AB1" s="148" t="s">
+      <c r="AB1" s="158" t="s">
         <v>67</v>
       </c>
-      <c r="AC1" s="148" t="s">
+      <c r="AC1" s="158" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:29" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="160" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
       <c r="P2" s="105" t="s">
         <v>69</v>
       </c>
@@ -3587,22 +3587,22 @@
       <c r="Z2" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="AA2" s="149"/>
-      <c r="AB2" s="149"/>
-      <c r="AC2" s="149"/>
+      <c r="AA2" s="159"/>
+      <c r="AB2" s="159"/>
+      <c r="AC2" s="159"/>
     </row>
     <row r="3" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="149" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="151"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149"/>
       <c r="K3" s="12"/>
       <c r="P3" s="109">
         <f>I6</f>
@@ -3658,15 +3658,15 @@
       </c>
     </row>
     <row r="4" spans="2:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="159"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
       <c r="K4" s="12"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
@@ -3689,11 +3689,11 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="153">
+      <c r="I6" s="151">
         <f>'Rescisão-RCA'!F16</f>
         <v>0</v>
       </c>
-      <c r="J6" s="153"/>
+      <c r="J6" s="151"/>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.2">
@@ -3709,33 +3709,33 @@
       <c r="K7" s="12"/>
     </row>
     <row r="9" spans="2:29" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="154" t="str">
+      <c r="B9" s="148" t="str">
         <f>"Declaro pelo presente, que recebí da empresa ÔMEGA DISTRIBUIDORA DE PRODUTOS ALIMENTÍCIOS LTDA, CNPJ 41.600.131/0002-78, estabelecida à Rua Capitão Hugo Bezerra, 120 - Barroso, a quantia destacada de "&amp;TEXT(VALUE(I6),"R$ #.##0,00_)")&amp;" ("&amp;AC3&amp;") como pagamento final de todas as importâncias a que fiz jus durante o período em que trabalhei na qualidade de Representante para a citada empresa."</f>
         <v>Declaro pelo presente, que recebí da empresa ÔMEGA DISTRIBUIDORA DE PRODUTOS ALIMENTÍCIOS LTDA, CNPJ 41.600.131/0002-78, estabelecida à Rua Capitão Hugo Bezerra, 120 - Barroso, a quantia destacada de R$ 0,00  () como pagamento final de todas as importâncias a que fiz jus durante o período em que trabalhei na qualidade de Representante para a citada empresa.</v>
       </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="148"/>
+      <c r="J9" s="148"/>
+      <c r="K9" s="148"/>
     </row>
     <row r="10" spans="2:29" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="154"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="154"/>
-      <c r="F10" s="154"/>
-      <c r="G10" s="154"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="154"/>
-      <c r="K10" s="154"/>
+      <c r="C10" s="148"/>
+      <c r="D10" s="148"/>
+      <c r="E10" s="148"/>
+      <c r="F10" s="148"/>
+      <c r="G10" s="148"/>
+      <c r="H10" s="148"/>
+      <c r="I10" s="148"/>
+      <c r="J10" s="148"/>
+      <c r="K10" s="148"/>
     </row>
     <row r="11" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
@@ -3746,18 +3746,18 @@
       <c r="E12" s="9"/>
     </row>
     <row r="14" spans="2:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="160" t="str">
+      <c r="B14" s="147" t="str">
         <f>"Fortaleza, " &amp; TEXT('Rescisão-RCA'!C10, "dd ""de"" mmmm ""de"" aaaa")</f>
         <v>Fortaleza, 00 de janeiro de 1900</v>
       </c>
-      <c r="C14" s="160"/>
-      <c r="D14" s="160"/>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
+      <c r="C14" s="147"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="147"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
+      <c r="H14" s="147"/>
+      <c r="I14" s="147"/>
+      <c r="J14" s="147"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
@@ -3793,29 +3793,29 @@
       <c r="J17" s="17"/>
     </row>
     <row r="18" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B18" s="159">
+      <c r="B18" s="146">
         <f>'Rescisão-RCA'!B5</f>
         <v>0</v>
       </c>
-      <c r="C18" s="159"/>
-      <c r="D18" s="159"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="146"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="159" t="s">
+      <c r="D19" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146"/>
+      <c r="H19" s="146"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
     </row>
@@ -3826,11 +3826,11 @@
       <c r="E20" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="152">
+      <c r="F20" s="150">
         <f>'Rescisão-RCA'!E5</f>
         <v>0</v>
       </c>
-      <c r="G20" s="152"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -3906,9 +3906,9 @@
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="158"/>
-      <c r="C27" s="158"/>
-      <c r="D27" s="158"/>
+      <c r="B27" s="145"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
@@ -3929,22 +3929,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="Q1:U1"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B4:J4"/>
     <mergeCell ref="B14:J14"/>
     <mergeCell ref="B18:J18"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="B2:K2"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
correções simples, planilhas datas 3
</commit_message>
<xml_diff>
--- a/rh/FORMULÁRIO DISTRATO RCA.xlsx
+++ b/rh/FORMULÁRIO DISTRATO RCA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Analista Comercial\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMERCIAL 04\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EF15C1-0D1F-4BD5-83B6-D2689956151B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8E1551-9DC0-4367-9CFD-42FC493EB1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rescisão-RCA" sheetId="13" r:id="rId1"/>
@@ -1734,9 +1734,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="172" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1781,6 +1778,45 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1788,45 +1824,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1848,6 +1845,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2773,7 +2773,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="53"/>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="134"/>
       <c r="E4" s="56" t="s">
         <v>6</v>
       </c>
@@ -2877,9 +2877,9 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="53"/>
-      <c r="B5" s="141"/>
-      <c r="C5" s="142"/>
-      <c r="D5" s="143"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="142"/>
       <c r="E5" s="130"/>
       <c r="F5" s="57"/>
       <c r="H5" s="36"/>
@@ -2921,13 +2921,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="53"/>
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
+      <c r="C7" s="135"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
       <c r="H7" s="120"/>
       <c r="I7" s="121"/>
       <c r="J7" s="120"/>
@@ -3232,11 +3232,11 @@
     </row>
     <row r="22" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="53"/>
-      <c r="B22" s="138" t="s">
+      <c r="B22" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="139"/>
-      <c r="D22" s="140"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="139"/>
       <c r="E22" s="53"/>
       <c r="F22" s="53"/>
       <c r="G22" s="10"/>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="31" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="53"/>
-      <c r="B31" s="133" t="str">
+      <c r="B31" s="165" t="str">
         <f>TEXT(C10, "dd ""de"" mmmm ""de"" aaaa")</f>
         <v>00 de janeiro de 1900</v>
       </c>
@@ -3393,8 +3393,8 @@
       <c r="B32" s="125"/>
       <c r="C32" s="127"/>
       <c r="D32" s="53"/>
-      <c r="E32" s="137"/>
-      <c r="F32" s="137"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="136"/>
       <c r="G32" s="10"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
@@ -3437,10 +3437,10 @@
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="53"/>
-      <c r="B37" s="144" t="s">
+      <c r="B37" s="143" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="144"/>
+      <c r="C37" s="143"/>
       <c r="D37" s="100"/>
       <c r="E37" s="101"/>
       <c r="F37" s="102"/>
@@ -3448,23 +3448,23 @@
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="53"/>
-      <c r="B38" s="134" t="s">
+      <c r="B38" s="133" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="134"/>
+      <c r="C38" s="133"/>
       <c r="D38" s="55"/>
-      <c r="E38" s="134"/>
-      <c r="F38" s="134"/>
+      <c r="E38" s="133"/>
+      <c r="F38" s="133"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="53"/>
-      <c r="B39" s="134" t="s">
+      <c r="B39" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="134"/>
+      <c r="C39" s="133"/>
       <c r="D39" s="55"/>
-      <c r="E39" s="134"/>
-      <c r="F39" s="134"/>
+      <c r="E39" s="133"/>
+      <c r="F39" s="133"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="53"/>
@@ -3489,6 +3489,9 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B31" unlockedFormula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
@@ -3517,43 +3520,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="Q1" s="152" t="s">
+      <c r="Q1" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="153"/>
-      <c r="S1" s="153"/>
-      <c r="T1" s="153"/>
-      <c r="U1" s="154"/>
-      <c r="V1" s="155" t="s">
+      <c r="R1" s="155"/>
+      <c r="S1" s="155"/>
+      <c r="T1" s="155"/>
+      <c r="U1" s="156"/>
+      <c r="V1" s="144" t="s">
         <v>65</v>
       </c>
-      <c r="W1" s="156"/>
-      <c r="X1" s="156"/>
-      <c r="Y1" s="156"/>
-      <c r="Z1" s="157"/>
-      <c r="AA1" s="158" t="s">
+      <c r="W1" s="145"/>
+      <c r="X1" s="145"/>
+      <c r="Y1" s="145"/>
+      <c r="Z1" s="146"/>
+      <c r="AA1" s="147" t="s">
         <v>66</v>
       </c>
-      <c r="AB1" s="158" t="s">
+      <c r="AB1" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="AC1" s="158" t="s">
+      <c r="AC1" s="147" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:29" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
       <c r="P2" s="105" t="s">
         <v>69</v>
       </c>
@@ -3587,22 +3590,22 @@
       <c r="Z2" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="AA2" s="159"/>
-      <c r="AB2" s="159"/>
-      <c r="AC2" s="159"/>
+      <c r="AA2" s="148"/>
+      <c r="AB2" s="148"/>
+      <c r="AC2" s="148"/>
     </row>
     <row r="3" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="149"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="149"/>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
       <c r="K3" s="12"/>
       <c r="P3" s="109">
         <f>I6</f>
@@ -3658,15 +3661,15 @@
       </c>
     </row>
     <row r="4" spans="2:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="146"/>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
       <c r="K4" s="12"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
@@ -3689,11 +3692,11 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="151">
+      <c r="I6" s="152">
         <f>'Rescisão-RCA'!F16</f>
         <v>0</v>
       </c>
-      <c r="J6" s="151"/>
+      <c r="J6" s="152"/>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.2">
@@ -3709,33 +3712,33 @@
       <c r="K7" s="12"/>
     </row>
     <row r="9" spans="2:29" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="148" t="str">
+      <c r="B9" s="153" t="str">
         <f>"Declaro pelo presente, que recebí da empresa ÔMEGA DISTRIBUIDORA DE PRODUTOS ALIMENTÍCIOS LTDA, CNPJ 41.600.131/0002-78, estabelecida à Rua Capitão Hugo Bezerra, 120 - Barroso, a quantia destacada de "&amp;TEXT(VALUE(I6),"R$ #.##0,00_)")&amp;" ("&amp;AC3&amp;") como pagamento final de todas as importâncias a que fiz jus durante o período em que trabalhei na qualidade de Representante para a citada empresa."</f>
         <v>Declaro pelo presente, que recebí da empresa ÔMEGA DISTRIBUIDORA DE PRODUTOS ALIMENTÍCIOS LTDA, CNPJ 41.600.131/0002-78, estabelecida à Rua Capitão Hugo Bezerra, 120 - Barroso, a quantia destacada de R$ 0,00  () como pagamento final de todas as importâncias a que fiz jus durante o período em que trabalhei na qualidade de Representante para a citada empresa.</v>
       </c>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
+      <c r="C9" s="153"/>
+      <c r="D9" s="153"/>
+      <c r="E9" s="153"/>
+      <c r="F9" s="153"/>
+      <c r="G9" s="153"/>
+      <c r="H9" s="153"/>
+      <c r="I9" s="153"/>
+      <c r="J9" s="153"/>
+      <c r="K9" s="153"/>
     </row>
     <row r="10" spans="2:29" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="148"/>
-      <c r="F10" s="148"/>
-      <c r="G10" s="148"/>
-      <c r="H10" s="148"/>
-      <c r="I10" s="148"/>
-      <c r="J10" s="148"/>
-      <c r="K10" s="148"/>
+      <c r="C10" s="153"/>
+      <c r="D10" s="153"/>
+      <c r="E10" s="153"/>
+      <c r="F10" s="153"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="153"/>
+      <c r="I10" s="153"/>
+      <c r="J10" s="153"/>
+      <c r="K10" s="153"/>
     </row>
     <row r="11" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
@@ -3746,18 +3749,18 @@
       <c r="E12" s="9"/>
     </row>
     <row r="14" spans="2:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="147" t="str">
+      <c r="B14" s="159" t="str">
         <f>"Fortaleza, " &amp; TEXT('Rescisão-RCA'!C10, "dd ""de"" mmmm ""de"" aaaa")</f>
         <v>Fortaleza, 00 de janeiro de 1900</v>
       </c>
-      <c r="C14" s="147"/>
-      <c r="D14" s="147"/>
-      <c r="E14" s="147"/>
-      <c r="F14" s="147"/>
-      <c r="G14" s="147"/>
-      <c r="H14" s="147"/>
-      <c r="I14" s="147"/>
-      <c r="J14" s="147"/>
+      <c r="C14" s="159"/>
+      <c r="D14" s="159"/>
+      <c r="E14" s="159"/>
+      <c r="F14" s="159"/>
+      <c r="G14" s="159"/>
+      <c r="H14" s="159"/>
+      <c r="I14" s="159"/>
+      <c r="J14" s="159"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
@@ -3793,29 +3796,29 @@
       <c r="J17" s="17"/>
     </row>
     <row r="18" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B18" s="146">
+      <c r="B18" s="158">
         <f>'Rescisão-RCA'!B5</f>
         <v>0</v>
       </c>
-      <c r="C18" s="146"/>
-      <c r="D18" s="146"/>
-      <c r="E18" s="146"/>
-      <c r="F18" s="146"/>
-      <c r="G18" s="146"/>
-      <c r="H18" s="146"/>
-      <c r="I18" s="146"/>
-      <c r="J18" s="146"/>
+      <c r="C18" s="158"/>
+      <c r="D18" s="158"/>
+      <c r="E18" s="158"/>
+      <c r="F18" s="158"/>
+      <c r="G18" s="158"/>
+      <c r="H18" s="158"/>
+      <c r="I18" s="158"/>
+      <c r="J18" s="158"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="146" t="s">
+      <c r="D19" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
-      <c r="H19" s="146"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
     </row>
@@ -3826,11 +3829,11 @@
       <c r="E20" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="150">
+      <c r="F20" s="151">
         <f>'Rescisão-RCA'!E5</f>
         <v>0</v>
       </c>
-      <c r="G20" s="150"/>
+      <c r="G20" s="151"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -3906,9 +3909,9 @@
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="145"/>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
@@ -3929,22 +3932,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="Q1:U1"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B4:J4"/>
     <mergeCell ref="B14:J14"/>
     <mergeCell ref="B18:J18"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="B2:K2"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3986,11 +3989,11 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="163"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="162"/>
     </row>
     <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
@@ -4070,12 +4073,12 @@
       <c r="D13" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="164" t="s">
+      <c r="E13" s="163" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="165"/>
-      <c r="G13" s="165"/>
-      <c r="H13" s="165"/>
+      <c r="F13" s="164"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="164"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="42" t="s">

</xml_diff>